<commit_message>
created snippets (markdown modules) for reuse
</commit_message>
<xml_diff>
--- a/docs/03-assets/processors-flow/FailureRetryHandling.xlsx
+++ b/docs/03-assets/processors-flow/FailureRetryHandling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrew/Documents/Work/layline/Dev/layline-doc/docs/03-assets/processors-flow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{76500F92-311C-3C40-9A76-AEA870877758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B5E7522-FBEF-FE47-92CA-E4D353BDDBBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12000" yWindow="5400" windowWidth="36420" windowHeight="17440" xr2:uid="{7C41F6BD-3115-B445-BA64-D896481BDC85}"/>
   </bookViews>
@@ -23,7 +23,7 @@
     <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$C$11</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$C$12:$C$16</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Retry #1</t>
   </si>
@@ -67,13 +67,22 @@
     <t>Retry #2</t>
   </si>
   <si>
-    <t>Time passed [ms]</t>
-  </si>
-  <si>
     <t>Setting</t>
   </si>
   <si>
     <t>Parameter</t>
+  </si>
+  <si>
+    <t>Retry #3</t>
+  </si>
+  <si>
+    <t>Retry #4</t>
+  </si>
+  <si>
+    <t>Retry #5</t>
+  </si>
+  <si>
+    <t>Time gap [ms]</t>
   </si>
 </sst>
 </file>
@@ -82,7 +91,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -131,7 +140,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -156,7 +165,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -183,10 +192,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="104"/>
+      <c14:style val="102"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="4"/>
+      <c:style val="2"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -197,21 +206,21 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" b="1"/>
-              <a:t>Time passed between retries [ms]</a:t>
+              <a:rPr lang="en-US"/>
+              <a:t>Time gap between retries [ms]</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -229,16 +238,16 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-DE"/>
@@ -249,19 +258,140 @@
     <c:plotArea>
       <c:layout/>
       <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
+              <c:f>Sheet1!$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Retry #1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-1DCB-7143-A2F7-2BB92B830907}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inBase"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
               <c:f>Sheet1!$C$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Time passed [ms]</c:v>
+                  <c:v>Time gap [ms]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1DCB-7143-A2F7-2BB92B830907}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Retry #2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -280,139 +410,449 @@
             <c:idx val="0"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time gap [ms]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>45000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000E-A674-524D-88DC-D415E535A2F2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Retry #3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="FF5721"/>
+                <a:schemeClr val="accent3"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
             <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000005-1DCB-7143-A2F7-2BB92B830907}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
               </c:ext>
             </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time gap [ms]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>80000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000F-A674-524D-88DC-D415E535A2F2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Retry #4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
           </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time gap [ms]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$15</c:f>
+              <c:numCache>
+                <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>115000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000010-A674-524D-88DC-D415E535A2F2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Retry #5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:dPt>
-            <c:idx val="1"/>
+            <c:idx val="0"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="FF5721"/>
+                <a:schemeClr val="accent5"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000004-1DCB-7143-A2F7-2BB92B830907}"/>
-              </c:ext>
-            </c:extLst>
           </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
+          <c:dLbls>
             <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FF5721"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:ln>
                 <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
             <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000001-1DCB-7143-A2F7-2BB92B830907}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
               </c:ext>
             </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FF5721"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000002-1DCB-7143-A2F7-2BB92B830907}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="4"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FF5721"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000003-1DCB-7143-A2F7-2BB92B830907}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$12:$B$16</c:f>
+              <c:f>Sheet1!$C$11</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Retry #1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Retry #2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Retry #2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Retry #2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Retry #2</c:v>
+                  <c:v>Time gap [ms]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$12:$C$16</c:f>
+              <c:f>Sheet1!$C$16</c:f>
               <c:numCache>
                 <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>10000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>45000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>80000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>115000</c:v>
-                </c:pt>
-                <c:pt idx="4">
                   <c:v>150000</c:v>
                 </c:pt>
               </c:numCache>
@@ -420,19 +860,20 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1DCB-7143-A2F7-2BB92B830907}"/>
+              <c16:uniqueId val="{00000011-A674-524D-88DC-D415E535A2F2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
+        <c:gapWidth val="150"/>
         <c:axId val="603066992"/>
         <c:axId val="603068720"/>
       </c:barChart>
@@ -441,45 +882,26 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-DE"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="603068720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
@@ -493,12 +915,12 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="l"/>
+        <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:schemeClr val="dk1">
                   <a:lumMod val="15000"/>
                   <a:lumOff val="85000"/>
                 </a:schemeClr>
@@ -514,8 +936,14 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
-            <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -524,9 +952,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
+                  <a:schemeClr val="dk1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
@@ -544,13 +972,54 @@
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
+        <a:pattFill prst="ltDnDiag">
+          <a:fgClr>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:fgClr>
+          <a:bgClr>
+            <a:schemeClr val="lt1"/>
+          </a:bgClr>
+        </a:pattFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
         <a:noFill/>
         <a:ln>
           <a:noFill/>
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-    </c:plotArea>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -564,11 +1033,11 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="bg1"/>
+      <a:schemeClr val="lt1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
+        <a:schemeClr val="dk1">
           <a:lumMod val="15000"/>
           <a:lumOff val="85000"/>
         </a:schemeClr>
@@ -596,31 +1065,65 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="15">
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
 </cs:colorStyle>
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="303">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -628,7 +1131,7 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -636,22 +1139,22 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="bg1"/>
+        <a:schemeClr val="lt1"/>
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -659,14 +1162,14 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="75000"/>
         <a:lumOff val="25000"/>
       </a:schemeClr>
@@ -703,35 +1206,45 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -743,30 +1256,34 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="15875">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -782,16 +1299,15 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -799,7 +1315,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="800" kern="1200"/>
   </cs:dataTable>
   <cs:downBar>
     <cs:lnRef idx="0"/>
@@ -811,17 +1327,18 @@
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -830,12 +1347,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
@@ -849,14 +1366,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -868,13 +1385,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
     </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
@@ -882,12 +1406,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -901,12 +1425,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="5000"/>
             <a:lumOff val="95000"/>
           </a:schemeClr>
@@ -920,31 +1444,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
@@ -952,58 +1457,18 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
@@ -1011,18 +1476,106 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1031,14 +1584,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -1047,7 +1599,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -1065,26 +1617,38 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -1092,13 +1656,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
     </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
@@ -1109,13 +1680,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>818263</xdr:colOff>
+      <xdr:colOff>818262</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>32927</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>754303</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>477212</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>69273</xdr:rowOff>
     </xdr:to>
@@ -1349,7 +1920,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F351CADC-123B-1443-8348-317DBE66E377}" name="Table2" displayName="Table2" ref="B11:C16" totalsRowShown="0">
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{E785A6D0-8760-9547-9EB3-DD3B8674B877}" name="Retries"/>
-    <tableColumn id="2" xr3:uid="{2433F199-CBE0-7C4D-91DC-D96694DA64C8}" name="Time passed [ms]" dataDxfId="0" dataCellStyle="Comma"/>
+    <tableColumn id="2" xr3:uid="{2433F199-CBE0-7C4D-91DC-D96694DA64C8}" name="Time gap [ms]" dataDxfId="0" dataCellStyle="Comma"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1654,8 +2225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEC65EDD-5E62-3D41-990D-96E4B2987995}">
   <dimension ref="B2:C16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="165" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="173" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1666,10 +2237,10 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
@@ -1710,7 +2281,7 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.2">
@@ -1733,7 +2304,7 @@
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C14" s="1">
         <f>C$4+(2*C$6)</f>
@@ -1742,7 +2313,7 @@
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C15" s="1">
         <f>C$4+(3*C$6)</f>
@@ -1751,7 +2322,7 @@
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C16" s="1">
         <f>C$4+(4*C$6)</f>

</xml_diff>